<commit_message>
GUI: Updated the Statistics and made minor cosmetic adjustments to the Update suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/_Test_Suite_Statistics_for_Folders.xlsx
+++ b/QA/Tests/CRUD/_Test_Suite_Statistics_for_Folders.xlsx
@@ -14,13 +14,14 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Total Ready to Write: </t>
   </si>
@@ -65,6 +66,9 @@
   </si>
   <si>
     <t>Create</t>
+  </si>
+  <si>
+    <t>Update</t>
   </si>
 </sst>
 </file>
@@ -249,6 +253,47 @@
         <row r="5">
           <cell r="G5">
             <v>3</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="E1">
+            <v>1</v>
+          </cell>
+          <cell r="G1">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="G4">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="G5">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -549,7 +594,7 @@
   <dimension ref="A1:J174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +636,7 @@
       </c>
       <c r="H1" s="4">
         <f>SUM($D:$D)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -668,9 +713,29 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <f>[3]Sheet1!$G$1</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <f>[3]Sheet1!$G$2</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <f>[3]Sheet1!$E$1</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <f>[3]Sheet1!$G$5</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <f>[3]Sheet1!$G$4</f>
+        <v>1</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="3"/>
@@ -684,7 +749,7 @@
       </c>
       <c r="H5" s="4">
         <f xml:space="preserve"> SUM($F:$F)</f>
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -710,7 +775,7 @@
       </c>
       <c r="H7" s="7">
         <f>H6/H5</f>
-        <v>0.68534482758620685</v>
+        <v>0.68240343347639487</v>
       </c>
       <c r="I7" s="3"/>
     </row>

</xml_diff>